<commit_message>
Changes made after 1st pre study data check
</commit_message>
<xml_diff>
--- a/experiments/Exp2/r_supportFiles/objects.xlsx
+++ b/experiments/Exp2/r_supportFiles/objects.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="objectSources" sheetId="1" r:id="rId1"/>
     <sheet name="randomisation" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="194">
   <si>
     <t>cardbox</t>
   </si>
@@ -594,12 +594,15 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>headphones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -953,16 +956,16 @@
       <selection activeCell="B89" sqref="A2:B89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -976,7 +979,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -987,7 +990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1009,7 +1012,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1020,7 +1023,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1072,7 +1075,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1080,7 +1083,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1116,7 +1119,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1127,7 +1130,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1138,7 +1141,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1171,7 +1174,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1193,7 +1196,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1231,7 +1234,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1303,7 +1306,7 @@
       </c>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1311,7 +1314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1322,7 +1325,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1347,7 +1350,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1361,7 +1364,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1375,7 +1378,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1386,7 +1389,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1419,7 +1422,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1430,7 +1433,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1438,7 +1441,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1449,7 +1452,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1468,7 +1471,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1482,7 +1485,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1493,7 +1496,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1507,7 +1510,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1530,7 +1533,7 @@
       </c>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1541,7 +1544,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1555,7 +1558,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1566,7 +1569,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1599,7 +1602,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1613,7 +1616,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1632,7 +1635,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1643,7 +1646,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -1665,7 +1668,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -1676,7 +1679,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -1690,7 +1693,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -1701,7 +1704,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -1712,7 +1715,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -1720,7 +1723,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -1731,7 +1734,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1753,7 +1756,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1761,7 +1764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -1786,7 +1789,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -1794,7 +1797,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -1802,7 +1805,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -1813,7 +1816,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -1824,7 +1827,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -1846,7 +1849,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -1857,7 +1860,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -1882,7 +1885,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -1893,7 +1896,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -1904,7 +1907,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -1918,7 +1921,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -1929,7 +1932,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -1943,15 +1946,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C90" s="2"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B104" s="1" t="s">
         <v>162</v>
       </c>
@@ -1959,22 +1962,22 @@
         <v>161</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B105" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B106" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B107" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
         <v>167</v>
       </c>
@@ -1982,7 +1985,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B109" s="1" t="s">
         <v>28</v>
       </c>
@@ -1990,7 +1993,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B110" s="1" t="s">
         <v>178</v>
       </c>
@@ -1998,7 +2001,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B111" s="1" t="s">
         <v>92</v>
       </c>
@@ -2009,7 +2012,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B112" s="1" t="s">
         <v>40</v>
       </c>
@@ -2017,7 +2020,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B113" s="1" t="s">
         <v>69</v>
       </c>
@@ -2028,7 +2031,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B114" s="1" t="s">
         <v>101</v>
       </c>
@@ -2036,7 +2039,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B115" s="1" t="s">
         <v>172</v>
       </c>
@@ -2044,7 +2047,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B116" s="1" t="s">
         <v>57</v>
       </c>
@@ -2052,12 +2055,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B118" s="1" t="s">
         <v>79</v>
       </c>
@@ -2065,7 +2068,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B119" s="1" t="s">
         <v>0</v>
       </c>
@@ -2116,16 +2119,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection sqref="A1:A88"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
-        <f ca="1">RAND()</f>
-        <v>0.14546081486461848</v>
+        <f t="shared" ref="A1:A32" ca="1" si="0">RAND()</f>
+        <v>0.31376947324578774</v>
       </c>
       <c r="B1" s="1">
         <v>47</v>
@@ -2134,10 +2137,10 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f ca="1">RAND()</f>
-        <v>0.77108607429926312</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.46897535469989349</v>
       </c>
       <c r="B2" s="1">
         <v>4</v>
@@ -2146,10 +2149,10 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f ca="1">RAND()</f>
-        <v>0.3767033917564504</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.37708170303350241</v>
       </c>
       <c r="B3" s="1">
         <v>39</v>
@@ -2158,10 +2161,10 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f ca="1">RAND()</f>
-        <v>9.5205811724583533E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.90411131218395013</v>
       </c>
       <c r="B4" s="1">
         <v>58</v>
@@ -2170,10 +2173,10 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f ca="1">RAND()</f>
-        <v>0.73682112915207221</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5.1505109117469527E-2</v>
       </c>
       <c r="B5" s="1">
         <v>35</v>
@@ -2182,10 +2185,10 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f ca="1">RAND()</f>
-        <v>0.70140120632100589</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.66333197177212189</v>
       </c>
       <c r="B6" s="1">
         <v>74</v>
@@ -2194,10 +2197,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f ca="1">RAND()</f>
-        <v>0.19953752341024222</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.36427955464902206</v>
       </c>
       <c r="B7" s="1">
         <v>44</v>
@@ -2206,10 +2209,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f ca="1">RAND()</f>
-        <v>0.77088237694662198</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.5197787283395785</v>
       </c>
       <c r="B8" s="1">
         <v>71</v>
@@ -2218,10 +2221,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f ca="1">RAND()</f>
-        <v>0.89116861978623196</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.37735654990975676</v>
       </c>
       <c r="B9" s="1">
         <v>70</v>
@@ -2230,10 +2233,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f ca="1">RAND()</f>
-        <v>0.78045438845609871</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.9826138677620526E-2</v>
       </c>
       <c r="B10" s="1">
         <v>69</v>
@@ -2242,10 +2245,10 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f ca="1">RAND()</f>
-        <v>0.21271483864494856</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.75695417801882892</v>
       </c>
       <c r="B11" s="1">
         <v>81</v>
@@ -2254,10 +2257,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f ca="1">RAND()</f>
-        <v>0.6326677427732802</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.90725810775188409</v>
       </c>
       <c r="B12" s="1">
         <v>77</v>
@@ -2266,10 +2269,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f ca="1">RAND()</f>
-        <v>0.51829846158895909</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.25426871229717518</v>
       </c>
       <c r="B13" s="1">
         <v>22</v>
@@ -2278,10 +2281,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f ca="1">RAND()</f>
-        <v>7.45371794824079E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.78439877711458561</v>
       </c>
       <c r="B14" s="1">
         <v>84</v>
@@ -2290,10 +2293,10 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f ca="1">RAND()</f>
-        <v>0.67713162650414838</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.88931037758498721</v>
       </c>
       <c r="B15" s="1">
         <v>27</v>
@@ -2302,10 +2305,10 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f ca="1">RAND()</f>
-        <v>1.2794773955710048E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.83633525118683916</v>
       </c>
       <c r="B16" s="1">
         <v>12</v>
@@ -2314,10 +2317,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f ca="1">RAND()</f>
-        <v>0.15811783187428219</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.60720682964705075</v>
       </c>
       <c r="B17" s="1">
         <v>73</v>
@@ -2326,10 +2329,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f ca="1">RAND()</f>
-        <v>0.85506154438462223</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.38531821983731729</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -2338,10 +2341,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f ca="1">RAND()</f>
-        <v>0.50140173067123173</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.58797468882098047</v>
       </c>
       <c r="B19" s="1">
         <v>8</v>
@@ -2350,10 +2353,10 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f ca="1">RAND()</f>
-        <v>0.38283651171183763</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.75295913763390609</v>
       </c>
       <c r="B20" s="1">
         <v>61</v>
@@ -2362,10 +2365,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f ca="1">RAND()</f>
-        <v>0.12748689871153329</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.80906983584931236</v>
       </c>
       <c r="B21" s="1">
         <v>46</v>
@@ -2374,10 +2377,10 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f ca="1">RAND()</f>
-        <v>0.43033063503405788</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.67248254478603786</v>
       </c>
       <c r="B22" s="1">
         <v>32</v>
@@ -2386,10 +2389,10 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f ca="1">RAND()</f>
-        <v>0.5397573068631627</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.2054234124684311</v>
       </c>
       <c r="B23" s="1">
         <v>43</v>
@@ -2398,10 +2401,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f ca="1">RAND()</f>
-        <v>0.1183736207193864</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.13998263674218359</v>
       </c>
       <c r="B24" s="1">
         <v>83</v>
@@ -2410,10 +2413,10 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f ca="1">RAND()</f>
-        <v>8.1601771656770739E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.68845166595439544</v>
       </c>
       <c r="B25" s="1">
         <v>64</v>
@@ -2422,10 +2425,10 @@
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f ca="1">RAND()</f>
-        <v>0.41785601536019901</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.36731627896100316</v>
       </c>
       <c r="B26" s="1">
         <v>53</v>
@@ -2434,10 +2437,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f ca="1">RAND()</f>
-        <v>0.70553203584375113</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.49534698452528214</v>
       </c>
       <c r="B27" s="1">
         <v>52</v>
@@ -2446,10 +2449,10 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
-        <f ca="1">RAND()</f>
-        <v>0.6284377830216058</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.73756729477583838</v>
       </c>
       <c r="B28" s="1">
         <v>30</v>
@@ -2458,10 +2461,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f ca="1">RAND()</f>
-        <v>0.66479144337224283</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.32121778183215643</v>
       </c>
       <c r="B29" s="1">
         <v>72</v>
@@ -2470,10 +2473,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
-        <f ca="1">RAND()</f>
-        <v>0.66079251185800214</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.34230730245023366</v>
       </c>
       <c r="B30" s="1">
         <v>86</v>
@@ -2482,10 +2485,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
-        <f ca="1">RAND()</f>
-        <v>0.5173133107860115</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.86034226244248668</v>
       </c>
       <c r="B31" s="1">
         <v>65</v>
@@ -2494,10 +2497,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
-        <f ca="1">RAND()</f>
-        <v>0.30357728363903447</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.27803763143646787</v>
       </c>
       <c r="B32" s="1">
         <v>17</v>
@@ -2506,10 +2509,10 @@
         <v>186</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
-        <f ca="1">RAND()</f>
-        <v>0.25439192179824288</v>
+        <f t="shared" ref="A33:A64" ca="1" si="1">RAND()</f>
+        <v>0.16572470391734984</v>
       </c>
       <c r="B33" s="1">
         <v>36</v>
@@ -2518,10 +2521,10 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
-        <f ca="1">RAND()</f>
-        <v>0.27381992282283818</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.38949264246447624</v>
       </c>
       <c r="B34" s="1">
         <v>5</v>
@@ -2530,10 +2533,10 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
-        <f ca="1">RAND()</f>
-        <v>0.33871292435754097</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6.3366894613056446E-2</v>
       </c>
       <c r="B35" s="1">
         <v>37</v>
@@ -2542,10 +2545,10 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
-        <f ca="1">RAND()</f>
-        <v>0.64428051254990137</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.79050471034592817</v>
       </c>
       <c r="B36" s="1">
         <v>63</v>
@@ -2554,10 +2557,10 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
-        <f ca="1">RAND()</f>
-        <v>0.39698804338480143</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.51671644344539347</v>
       </c>
       <c r="B37" s="1">
         <v>15</v>
@@ -2566,10 +2569,10 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
-        <f ca="1">RAND()</f>
-        <v>0.19125893406995242</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.3336128180183158E-2</v>
       </c>
       <c r="B38" s="1">
         <v>76</v>
@@ -2578,10 +2581,10 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
-        <f ca="1">RAND()</f>
-        <v>0.83152981436833939</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.53452848011634246</v>
       </c>
       <c r="B39" s="1">
         <v>51</v>
@@ -2590,10 +2593,10 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f ca="1">RAND()</f>
-        <v>0.26616375500231448</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.69773331631498126</v>
       </c>
       <c r="B40" s="1">
         <v>79</v>
@@ -2602,10 +2605,10 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
-        <f ca="1">RAND()</f>
-        <v>0.70679243827153093</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.3055759566858246</v>
       </c>
       <c r="B41" s="1">
         <v>29</v>
@@ -2614,10 +2617,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
-        <f ca="1">RAND()</f>
-        <v>0.64852931015823068</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.82832713446959028</v>
       </c>
       <c r="B42" s="1">
         <v>80</v>
@@ -2626,10 +2629,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
-        <f ca="1">RAND()</f>
-        <v>0.35885259576719641</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.11686976494093271</v>
       </c>
       <c r="B43" s="1">
         <v>26</v>
@@ -2638,10 +2641,10 @@
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
-        <f ca="1">RAND()</f>
-        <v>0.38928352677176137</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.58667790974971235</v>
       </c>
       <c r="B44" s="1">
         <v>87</v>
@@ -2650,10 +2653,10 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
-        <f ca="1">RAND()</f>
-        <v>0.7619472297185178</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.25906143674704829</v>
       </c>
       <c r="B45" s="1">
         <v>85</v>
@@ -2662,10 +2665,10 @@
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
-        <f ca="1">RAND()</f>
-        <v>0.63233105904198139</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.26480014411111641</v>
       </c>
       <c r="B46" s="1">
         <v>28</v>
@@ -2674,10 +2677,10 @@
         <v>163</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
-        <f ca="1">RAND()</f>
-        <v>0.85094314991072251</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.69289035847563563</v>
       </c>
       <c r="B47" s="1">
         <v>33</v>
@@ -2686,10 +2689,10 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
-        <f ca="1">RAND()</f>
-        <v>0.95324690233992138</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.70263400460424408</v>
       </c>
       <c r="B48" s="1">
         <v>24</v>
@@ -2698,10 +2701,10 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
-        <f ca="1">RAND()</f>
-        <v>0.23024316011541668</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.11606096769409491</v>
       </c>
       <c r="B49" s="1">
         <v>56</v>
@@ -2710,10 +2713,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
-        <f ca="1">RAND()</f>
-        <v>0.23466597110556031</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.93005930992118857</v>
       </c>
       <c r="B50" s="1">
         <v>50</v>
@@ -2722,10 +2725,10 @@
         <v>190</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
-        <f ca="1">RAND()</f>
-        <v>0.70287786549312792</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.49594862383080229</v>
       </c>
       <c r="B51" s="1">
         <v>49</v>
@@ -2734,10 +2737,10 @@
         <v>165</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
-        <f ca="1">RAND()</f>
-        <v>0.50343408978121229</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.90477766098663837</v>
       </c>
       <c r="B52" s="1">
         <v>31</v>
@@ -2746,10 +2749,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
-        <f ca="1">RAND()</f>
-        <v>0.52248069319587953</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.61695891879993503</v>
       </c>
       <c r="B53" s="1">
         <v>1</v>
@@ -2758,10 +2761,10 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
-        <f ca="1">RAND()</f>
-        <v>6.9536080086689878E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.22299896928074514</v>
       </c>
       <c r="B54" s="1">
         <v>59</v>
@@ -2770,22 +2773,22 @@
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
-        <f ca="1">RAND()</f>
-        <v>0.75778820990005269</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.17152692357517441</v>
       </c>
       <c r="B55" s="1">
         <v>45</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
-        <f ca="1">RAND()</f>
-        <v>0.87473295352914382</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.66212206815942443</v>
       </c>
       <c r="B56" s="1">
         <v>48</v>
@@ -2794,10 +2797,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
-        <f ca="1">RAND()</f>
-        <v>0.47056632124005959</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.16079813729389314</v>
       </c>
       <c r="B57" s="1">
         <v>20</v>
@@ -2806,10 +2809,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
-        <f ca="1">RAND()</f>
-        <v>0.33009940995208376</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.51073272599847452</v>
       </c>
       <c r="B58" s="1">
         <v>10</v>
@@ -2818,10 +2821,10 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
-        <f ca="1">RAND()</f>
-        <v>0.85472822439247753</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.60691388735459806</v>
       </c>
       <c r="B59" s="1">
         <v>40</v>
@@ -2830,10 +2833,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
-        <f ca="1">RAND()</f>
-        <v>0.27304698316178133</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.38474330502605625</v>
       </c>
       <c r="B60" s="1">
         <v>18</v>
@@ -2842,10 +2845,10 @@
         <v>157</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
-        <f ca="1">RAND()</f>
-        <v>0.81859556223681573</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.46958423337762356</v>
       </c>
       <c r="B61" s="1">
         <v>60</v>
@@ -2854,10 +2857,10 @@
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
-        <f ca="1">RAND()</f>
-        <v>0.69125546792173131</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.92203797913727781</v>
       </c>
       <c r="B62" s="1">
         <v>41</v>
@@ -2866,10 +2869,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
-        <f ca="1">RAND()</f>
-        <v>0.43109035987441824</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.27839115693808936</v>
       </c>
       <c r="B63" s="1">
         <v>25</v>
@@ -2878,10 +2881,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
-        <f ca="1">RAND()</f>
-        <v>0.11065557129448167</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.98948755365350183</v>
       </c>
       <c r="B64" s="1">
         <v>62</v>
@@ -2890,10 +2893,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
-        <f ca="1">RAND()</f>
-        <v>0.38250347754408309</v>
+        <f t="shared" ref="A65:A88" ca="1" si="2">RAND()</f>
+        <v>0.4696962084405083</v>
       </c>
       <c r="B65" s="1">
         <v>82</v>
@@ -2902,10 +2905,10 @@
         <v>160</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
-        <f ca="1">RAND()</f>
-        <v>0.32614911762069598</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.16665333238315827</v>
       </c>
       <c r="B66" s="1">
         <v>66</v>
@@ -2914,10 +2917,10 @@
         <v>155</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
-        <f ca="1">RAND()</f>
-        <v>0.75161586177317719</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.84948226248871994</v>
       </c>
       <c r="B67" s="1">
         <v>67</v>
@@ -2926,10 +2929,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
-        <f ca="1">RAND()</f>
-        <v>1.9809433767254969E-3</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.8231567613493369E-2</v>
       </c>
       <c r="B68" s="1">
         <v>3</v>
@@ -2938,10 +2941,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
-        <f ca="1">RAND()</f>
-        <v>0.64745328852294737</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.84702222672277427</v>
       </c>
       <c r="B69" s="1">
         <v>34</v>
@@ -2950,10 +2953,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
-        <f ca="1">RAND()</f>
-        <v>0.98440574765009814</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.44896432307054102</v>
       </c>
       <c r="B70" s="1">
         <v>16</v>
@@ -2962,10 +2965,10 @@
         <v>171</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
-        <f ca="1">RAND()</f>
-        <v>0.47972344542273393</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.76716549071030604</v>
       </c>
       <c r="B71" s="1">
         <v>23</v>
@@ -2974,10 +2977,10 @@
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
-        <f ca="1">RAND()</f>
-        <v>0.74433930430313611</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.70169287825202165</v>
       </c>
       <c r="B72" s="1">
         <v>57</v>
@@ -2986,10 +2989,10 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
-        <f ca="1">RAND()</f>
-        <v>0.89807061823511425</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.51787108578484342</v>
       </c>
       <c r="B73" s="1">
         <v>55</v>
@@ -2998,10 +3001,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
-        <f ca="1">RAND()</f>
-        <v>0.2797109311479431</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.44725556320445292</v>
       </c>
       <c r="B74" s="1">
         <v>21</v>
@@ -3010,10 +3013,10 @@
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
-        <f ca="1">RAND()</f>
-        <v>0.66237105587242262</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.50778028093051641</v>
       </c>
       <c r="B75" s="1">
         <v>75</v>
@@ -3022,10 +3025,10 @@
         <v>168</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
-        <f ca="1">RAND()</f>
-        <v>0.56966723902972416</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.5222394747571919</v>
       </c>
       <c r="B76" s="1">
         <v>54</v>
@@ -3034,10 +3037,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
-        <f ca="1">RAND()</f>
-        <v>0.30383352436364286</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.73402482915701139</v>
       </c>
       <c r="B77" s="1">
         <v>14</v>
@@ -3046,10 +3049,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
-        <f ca="1">RAND()</f>
-        <v>0.38734782126697587</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.55098876452038559</v>
       </c>
       <c r="B78" s="1">
         <v>2</v>
@@ -3058,10 +3061,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
-        <f ca="1">RAND()</f>
-        <v>0.8794048886117487</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.51026777962275216</v>
       </c>
       <c r="B79" s="1">
         <v>68</v>
@@ -3070,10 +3073,10 @@
         <v>63</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
-        <f ca="1">RAND()</f>
-        <v>0.3072321422708103</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.10303427516659813</v>
       </c>
       <c r="B80" s="1">
         <v>13</v>
@@ -3082,10 +3085,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
-        <f ca="1">RAND()</f>
-        <v>0.20632427179260659</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.22460086381161237</v>
       </c>
       <c r="B81" s="1">
         <v>19</v>
@@ -3094,10 +3097,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82">
-        <f ca="1">RAND()</f>
-        <v>0.60121153262801985</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.45908466034907591</v>
       </c>
       <c r="B82" s="1">
         <v>7</v>
@@ -3106,10 +3109,10 @@
         <v>97</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83">
-        <f ca="1">RAND()</f>
-        <v>0.60395511233849086</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.71414302600916102</v>
       </c>
       <c r="B83" s="1">
         <v>9</v>
@@ -3118,10 +3121,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84">
-        <f ca="1">RAND()</f>
-        <v>0.76193822211262774</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.36710617656987088</v>
       </c>
       <c r="B84" s="1">
         <v>11</v>
@@ -3130,10 +3133,10 @@
         <v>128</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85">
-        <f ca="1">RAND()</f>
-        <v>0.93192367635665874</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.94804810778775717</v>
       </c>
       <c r="B85" s="1">
         <v>6</v>
@@ -3142,10 +3145,10 @@
         <v>184</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86">
-        <f ca="1">RAND()</f>
-        <v>0.21686706955553714</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.6613343722475612</v>
       </c>
       <c r="B86" s="1">
         <v>38</v>
@@ -3154,10 +3157,10 @@
         <v>188</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87">
-        <f ca="1">RAND()</f>
-        <v>0.65911067808355472</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.53800244423724719</v>
       </c>
       <c r="B87" s="1">
         <v>42</v>
@@ -3166,10 +3169,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88">
-        <f ca="1">RAND()</f>
-        <v>0.49710185636182624</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.24992217071716183</v>
       </c>
       <c r="B88" s="1">
         <v>78</v>

</xml_diff>